<commit_message>
Added AdminSearchData tab to TestData.xlsx
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/TestData.xlsx
+++ b/src/main/java/testdata/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anilkumarb\Documents\Truckstop-RATE 5-4-2018\Truckstop-RATE\src\main\java\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumAutomation\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" firstSheet="18" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" firstSheet="17" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="BrokerLoginData" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,8 @@
     <sheet name="BrokerBankingData" sheetId="15" r:id="rId18"/>
     <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId19"/>
     <sheet name="CarrierBankingData" sheetId="16" r:id="rId20"/>
-    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId21"/>
-    <sheet name="AdminLogin" sheetId="9" r:id="rId22"/>
+    <sheet name="AdminLogin" sheetId="9" r:id="rId21"/>
+    <sheet name="AdminSearchData" sheetId="25" r:id="rId22"/>
     <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId23"/>
     <sheet name="tasks" sheetId="3" state="hidden" r:id="rId24"/>
   </sheets>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="155">
   <si>
     <t>Username</t>
   </si>
@@ -256,12 +256,6 @@
     <t>brokerregisterstage1@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>unmatched99@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>unmatched90@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>Search Payer</t>
   </si>
   <si>
@@ -409,18 +403,12 @@
     <t>FuelSurcharge</t>
   </si>
   <si>
-    <t>unmatchedCVK06202018C@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>07/24/2018</t>
   </si>
   <si>
     <t>2468.15</t>
   </si>
   <si>
-    <t>60202018C</t>
-  </si>
-  <si>
     <t>06/12/2018</t>
   </si>
   <si>
@@ -478,25 +466,55 @@
     <t>275</t>
   </si>
   <si>
-    <t>carrier81@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>carrier82@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>brokerregister29@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>carrierregister58@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>Search InvoiceNumber</t>
-  </si>
-  <si>
-    <t>Payer</t>
-  </si>
-  <si>
-    <t>broker registration</t>
+    <t>brokerregister94@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>carrierregister45@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>unmatched80@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>unmatched81@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>carrierregister99@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>PaymentID</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>FilterByAll</t>
+  </si>
+  <si>
+    <t>FilterByUnmatched</t>
+  </si>
+  <si>
+    <t>FilterByNotScheduled</t>
+  </si>
+  <si>
+    <t>FilterByScheduled</t>
+  </si>
+  <si>
+    <t>FilterByPaid</t>
+  </si>
+  <si>
+    <t>FilterByError</t>
+  </si>
+  <si>
+    <t>FilterByCanceled</t>
+  </si>
+  <si>
+    <t>AmountFrom</t>
+  </si>
+  <si>
+    <t>AmountTo</t>
   </si>
 </sst>
 </file>
@@ -504,7 +522,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -538,7 +556,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,8 +581,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -598,13 +622,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -629,6 +698,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -948,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -965,90 +1037,90 @@
         <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>29</v>
@@ -1057,87 +1129,87 @@
         <v>456789</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="4">
+        <v>7099</v>
+      </c>
+      <c r="G2" s="4">
+        <v>7099</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>124</v>
       </c>
       <c r="J2" s="16" t="b">
         <v>1</v>
       </c>
       <c r="K2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="P2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="V2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="W2" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="X2" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="Y2" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="Z2" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA2" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="AB2" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="AC2" s="16" t="s">
         <v>137</v>
-      </c>
-      <c r="Y2" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="AA2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" display="unmatchedCVK06202018C@loadpaytest.truckstop.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1145,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1177,36 +1249,18 @@
         <v>142</v>
       </c>
       <c r="B2" s="4">
-        <v>709813</v>
+        <v>7099</v>
       </c>
       <c r="C2" s="4">
-        <v>709813</v>
+        <v>7099</v>
       </c>
       <c r="D2" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3" s="4">
-        <v>709814</v>
-      </c>
-      <c r="C3" s="4">
-        <v>709814</v>
-      </c>
-      <c r="D3" s="4">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1226,10 +1280,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1261,10 +1315,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1322,7 +1376,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1353,13 +1407,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="B2" s="4">
-        <v>10041598</v>
+        <v>1004151</v>
       </c>
       <c r="C2" s="4">
-        <v>10041598</v>
+        <v>1004151</v>
       </c>
       <c r="D2" s="4">
         <v>10</v>
@@ -1373,13 +1427,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="B3" s="4">
-        <v>10041599</v>
+        <v>1004152</v>
       </c>
       <c r="C3" s="4">
-        <v>10041599</v>
+        <v>1004152</v>
       </c>
       <c r="D3" s="4">
         <v>10</v>
@@ -1765,7 +1819,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1786,33 +1840,33 @@
         <v>63</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2" s="4">
         <v>123.45</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F2" s="4">
         <v>61420181</v>
@@ -1917,72 +1971,6 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.625" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="4">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1132860</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1132860</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2009,6 +1997,78 @@
       </c>
       <c r="B2" s="4" t="s">
         <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>32922</v>
       </c>
     </row>
   </sheetData>
@@ -2156,10 +2216,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -2232,7 +2292,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>64</v>
@@ -2269,18 +2329,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2317,10 +2377,10 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2328,13 +2388,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2364,30 +2424,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2521,10 +2581,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Commit for reset password
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/TestData.xlsx
+++ b/src/main/java/testdata/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumAutomation\LoadPay-Truckstop\SeleniumAutomation\src\main\java\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumAutomation\LoadPay-Truckstop\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12975" windowHeight="4020" tabRatio="500" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12972" windowHeight="4020" tabRatio="500" firstSheet="21" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="BrokerLoginData" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,10 @@
     <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId21"/>
     <sheet name="AdminLogin" sheetId="9" r:id="rId22"/>
     <sheet name="AdminSearchData" sheetId="26" r:id="rId23"/>
-    <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId24"/>
-    <sheet name="tasks" sheetId="3" state="hidden" r:id="rId25"/>
+    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId24"/>
+    <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId25"/>
+    <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId26"/>
+    <sheet name="tasks" sheetId="3" state="hidden" r:id="rId27"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="173">
   <si>
     <t>Username</t>
   </si>
@@ -543,6 +545,33 @@
   </si>
   <si>
     <t>02/01/2018</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>CurrentPassword</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>ConfirmNewPassword</t>
+  </si>
+  <si>
+    <t>yuriibrokerstage@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>Password@7</t>
+  </si>
+  <si>
+    <t>Password@12</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yuriibrokerstage@loadpaytest.truckstop.com </t>
   </si>
 </sst>
 </file>
@@ -550,9 +579,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -583,8 +612,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -621,6 +663,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -790,12 +837,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -836,9 +884,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1124,13 +1176,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1138,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>67</v>
       </c>
@@ -1159,12 +1211,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>62</v>
       </c>
@@ -1253,7 +1305,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
@@ -1354,18 +1406,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.875" customWidth="1"/>
+    <col min="1" max="1" width="35.8984375" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -1379,7 +1431,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>88</v>
       </c>
@@ -1410,13 +1462,13 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>89</v>
       </c>
@@ -1424,7 +1476,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>100</v>
       </c>
@@ -1445,13 +1497,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>89</v>
       </c>
@@ -1459,7 +1511,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>500</v>
       </c>
@@ -1480,15 +1532,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -1496,7 +1548,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>55</v>
       </c>
@@ -1517,13 +1569,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1543,7 +1595,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -1563,7 +1615,7 @@
         <v>295676689</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -1600,16 +1652,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="35.19921875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1674,7 +1726,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>20</v>
@@ -1754,19 +1806,19 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.09765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.8984375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1831,7 +1883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>48</v>
@@ -1911,15 +1963,15 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -1933,7 +1985,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>60</v>
       </c>
@@ -1960,17 +2012,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>62</v>
       </c>
@@ -1990,7 +2042,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>76</v>
       </c>
@@ -2028,13 +2080,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2042,7 +2094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2066,15 +2118,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -2088,7 +2140,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
@@ -2115,17 +2167,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.625" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.59765625" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>62</v>
       </c>
@@ -2145,7 +2197,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>88</v>
       </c>
@@ -2181,13 +2233,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
@@ -2195,7 +2247,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
@@ -2216,23 +2268,23 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
         <v>148</v>
       </c>
@@ -2270,7 +2322,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="33">
         <v>32002</v>
       </c>
@@ -2300,7 +2352,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="25"/>
       <c r="B3" s="18">
         <v>100</v>
@@ -2332,7 +2384,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="25"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2364,7 +2416,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="25"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2392,7 +2444,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2420,7 +2472,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="25"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -2448,7 +2500,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="25"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2476,7 +2528,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="25"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2504,7 +2556,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2532,7 +2584,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2560,7 +2612,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
         <v>33343</v>
       </c>
@@ -2590,7 +2642,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
         <v>33310</v>
       </c>
@@ -2620,7 +2672,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="25">
         <v>33558</v>
       </c>
@@ -2650,7 +2702,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
         <v>33280</v>
       </c>
@@ -2680,7 +2732,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="25">
         <v>33307</v>
       </c>
@@ -2710,7 +2762,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28">
         <v>8140</v>
       </c>
@@ -2748,19 +2800,131 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" customWidth="1"/>
+    <col min="4" max="4" width="17.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.296875" customWidth="1"/>
+    <col min="3" max="3" width="20.69921875" customWidth="1"/>
+    <col min="4" max="4" width="25.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2768,7 +2932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2786,13 +2950,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2806,26 +2970,26 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
-    <col min="4" max="4" width="35.75" customWidth="1"/>
-    <col min="5" max="5" width="36.375" customWidth="1"/>
-    <col min="6" max="6" width="12.875" customWidth="1"/>
-    <col min="9" max="9" width="11.875" customWidth="1"/>
-    <col min="10" max="10" width="12.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="15.25" customWidth="1"/>
-    <col min="13" max="13" width="14.75" customWidth="1"/>
-    <col min="14" max="14" width="15.875" customWidth="1"/>
-    <col min="15" max="15" width="15.25" customWidth="1"/>
-    <col min="16" max="16" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="14.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.09765625" customWidth="1"/>
+    <col min="3" max="3" width="17.8984375" customWidth="1"/>
+    <col min="4" max="4" width="35.69921875" customWidth="1"/>
+    <col min="5" max="5" width="36.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.8984375" customWidth="1"/>
+    <col min="9" max="9" width="11.8984375" customWidth="1"/>
+    <col min="10" max="10" width="12.09765625" customWidth="1"/>
+    <col min="11" max="11" width="14.3984375" customWidth="1"/>
+    <col min="12" max="12" width="15.19921875" customWidth="1"/>
+    <col min="13" max="13" width="14.69921875" customWidth="1"/>
+    <col min="14" max="14" width="15.8984375" customWidth="1"/>
+    <col min="15" max="15" width="15.19921875" customWidth="1"/>
+    <col min="16" max="16" width="16.19921875" customWidth="1"/>
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2878,7 +3042,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2946,13 +3110,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.125" customWidth="1"/>
+    <col min="1" max="1" width="36.09765625" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2960,7 +3124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>88</v>
       </c>
@@ -2985,13 +3149,13 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3002,7 +3166,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -3029,15 +3193,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8984375" customWidth="1"/>
     <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -3051,7 +3215,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -3082,15 +3246,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>84</v>
       </c>
@@ -3104,7 +3268,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>91</v>
       </c>
@@ -3137,13 +3301,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>50</v>
       </c>
@@ -3151,7 +3315,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>6542988</v>
       </c>
@@ -3173,22 +3337,22 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="13.69921875" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="35.875" customWidth="1"/>
+    <col min="5" max="5" width="35.8984375" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="11" max="12" width="14.625" customWidth="1"/>
+    <col min="11" max="12" width="14.59765625" customWidth="1"/>
     <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="15" max="15" width="13.75" customWidth="1"/>
-    <col min="16" max="16" width="12.625" customWidth="1"/>
+    <col min="15" max="15" width="13.69921875" customWidth="1"/>
+    <col min="16" max="16" width="12.59765625" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -3241,7 +3405,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>

</xml_diff>